<commit_message>
fix: no POD column in 3 mavo template
</commit_message>
<xml_diff>
--- a/pta-template-3mavo.xlsx
+++ b/pta-template-3mavo.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_11FA35FCE2C2274F79E11ADB5EDE0F4A6A6A2125" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59D8ED10-8F77-4D45-8384-F2373FECDED8}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leidenuniv1-my.sharepoint.com/personal/s4490932_vuw_leidenuniv_nl/Documents/PTA Platform Templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_11FA35FCE2C2274F79E11ADB5EDE0F4A6A6A2125" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AE0D7E-942F-413D-A280-22F2F6B29B40}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>{{name}}</t>
   </si>
@@ -113,6 +118,9 @@
 (cijfers invullen)</t>
   </si>
   <si>
+    <t>POD</t>
+  </si>
+  <si>
     <t>PTA</t>
   </si>
   <si>
@@ -144,6 +152,9 @@
   </si>
   <si>
     <t>{{test.resitable}}</t>
+  </si>
+  <si>
+    <t>{{test.pod_weight}}</t>
   </si>
   <si>
     <t>{{test.pta_weight}}</t>
@@ -288,7 +299,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -366,6 +377,10 @@
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -387,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -512,6 +527,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -574,55 +598,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,6 +703,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -881,39 +911,39 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AP61"/>
+  <dimension ref="A1:AO61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.53515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.53515625" customWidth="1"/>
+    <col min="4" max="4" width="18.3828125" customWidth="1"/>
+    <col min="5" max="5" width="13.53515625" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.53515625" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" customWidth="1"/>
-    <col min="16" max="41" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.15234375" customWidth="1"/>
+    <col min="11" max="11" width="10.3828125" customWidth="1"/>
+    <col min="12" max="12" width="6.53515625" customWidth="1"/>
+    <col min="14" max="14" width="13.84375" customWidth="1"/>
+    <col min="15" max="15" width="18.15234375" customWidth="1"/>
+    <col min="16" max="41" width="12.53515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="36" customHeight="1">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:41" ht="36" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -992,13 +1022,13 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="2" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+    <row r="2" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1053,14 +1083,14 @@
       <c r="AN2" s="3"/>
       <c r="AO2" s="3"/>
     </row>
-    <row r="3" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1116,14 +1146,14 @@
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
     </row>
-    <row r="4" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A4" s="42" t="s">
+    <row r="4" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1179,12 +1209,12 @@
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
     </row>
-    <row r="5" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+    <row r="5" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="34"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1238,25 +1268,25 @@
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
     </row>
-    <row r="6" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="37" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="25" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="41"/>
+      <c r="J6" s="30"/>
       <c r="K6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1307,16 +1337,16 @@
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
     </row>
-    <row r="7" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="1"/>
@@ -1364,7 +1394,7 @@
       <c r="AN7" s="3"/>
       <c r="AO7" s="3"/>
     </row>
-    <row r="8" spans="1:41" ht="129.75" customHeight="1">
+    <row r="8" spans="1:41" ht="129.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -1377,12 +1407,12 @@
       <c r="D8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="17" t="s">
         <v>18</v>
       </c>
@@ -1395,10 +1425,10 @@
       <c r="L8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="28"/>
+      <c r="N8" s="42"/>
       <c r="O8" s="17" t="s">
         <v>23</v>
       </c>
@@ -1439,30 +1469,32 @@
       <c r="AN8" s="3"/>
       <c r="AO8" s="3"/>
     </row>
-    <row r="9" spans="1:41" ht="24" customHeight="1">
+    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="41"/>
+      <c r="N9" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -1494,43 +1526,45 @@
       <c r="AN9" s="3"/>
       <c r="AO9" s="3"/>
     </row>
-    <row r="10" spans="1:41" ht="57.75">
+    <row r="10" spans="1:41" ht="58.3" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="24"/>
+      <c r="E10" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="M10" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="47" t="s">
+        <v>37</v>
+      </c>
       <c r="O10" s="21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="2" t="s">
@@ -1563,7 +1597,7 @@
       <c r="AN10" s="3"/>
       <c r="AO10" s="3"/>
     </row>
-    <row r="11" spans="1:41" ht="15.75" customHeight="1">
+    <row r="11" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1581,24 +1615,24 @@
       <c r="O11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X11" s="3">
         <v>7</v>
       </c>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A12" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="E12" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+    <row r="12" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="E12" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1609,27 +1643,27 @@
       <c r="O12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X12" s="3">
         <v>8</v>
       </c>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:41" ht="12.75">
+    <row r="13" spans="1:41" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="24"/>
+        <v>42</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="28"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1641,27 +1675,27 @@
       <c r="O13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X13" s="3">
         <v>9</v>
       </c>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:41" ht="25.5">
+    <row r="14" spans="1:41" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="28"/>
       <c r="E14" s="15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1673,19 +1707,19 @@
       <c r="O14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X14" s="3">
         <v>10</v>
       </c>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:41" ht="12.75">
+    <row r="15" spans="1:41" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="24"/>
+        <v>49</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="28"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1699,19 +1733,19 @@
       <c r="O15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:41" ht="12.75">
+    <row r="16" spans="1:41" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="28"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1725,19 +1759,19 @@
       <c r="O16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X16" s="3">
         <v>12</v>
       </c>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" ht="12.75">
+    <row r="17" spans="1:25" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="28"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1751,19 +1785,19 @@
       <c r="O17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X17" s="3">
         <v>13</v>
       </c>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25" ht="12.75">
+    <row r="18" spans="1:25" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="28"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -1777,19 +1811,19 @@
       <c r="O18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X18" s="3">
         <v>14</v>
       </c>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" ht="12.75">
+    <row r="19" spans="1:25" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="24"/>
+        <v>54</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="1"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
@@ -1804,19 +1838,19 @@
       <c r="O19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X19" s="11">
         <v>15</v>
       </c>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" ht="12.75">
+    <row r="20" spans="1:25" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="1"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -1832,12 +1866,12 @@
       <c r="V20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" ht="12.75">
+    <row r="21" spans="1:25" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="1"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1853,30 +1887,30 @@
       <c r="V21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="29" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" spans="1:25" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O29" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O30" s="12">
         <v>401</v>
       </c>
@@ -1890,21 +1924,21 @@
         <v>46</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O31" s="12">
         <v>402</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q31" s="1">
         <v>38</v>
@@ -1913,21 +1947,21 @@
         <v>47</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O32" s="12">
         <v>403</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q32" s="1">
         <v>39</v>
@@ -1936,14 +1970,14 @@
         <v>48</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T32" s="1"/>
       <c r="U32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O33" s="12">
         <v>404</v>
       </c>
@@ -1955,14 +1989,14 @@
         <v>49</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O34" s="12">
         <v>405</v>
       </c>
@@ -1974,14 +2008,14 @@
         <v>50</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O35" s="12">
         <v>406</v>
       </c>
@@ -1993,27 +2027,27 @@
         <v>51</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="36" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O36" s="12">
         <v>407</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
     </row>
-    <row r="37" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="37" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O37" s="12">
         <v>408</v>
       </c>
@@ -2024,11 +2058,11 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="38" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O38" s="12">
         <v>409</v>
       </c>
@@ -2039,11 +2073,11 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="U38" s="1"/>
     </row>
-    <row r="39" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="39" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O39" s="12">
         <v>410</v>
       </c>
@@ -2054,11 +2088,11 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="40" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O40" s="12">
         <v>411</v>
       </c>
@@ -2069,11 +2103,11 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="U40" s="1"/>
     </row>
-    <row r="41" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="41" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O41" s="12">
         <v>412</v>
       </c>
@@ -2084,11 +2118,11 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="U41" s="1"/>
     </row>
-    <row r="42" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O42" s="12">
         <v>413</v>
       </c>
@@ -2101,20 +2135,20 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
     </row>
-    <row r="43" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="43" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O43" s="12">
         <v>414</v>
       </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
     </row>
-    <row r="44" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="44" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O44" s="3"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1">
@@ -2125,7 +2159,7 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
     </row>
-    <row r="45" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="45" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O45" s="3"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1">
@@ -2136,7 +2170,7 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
     </row>
-    <row r="46" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="46" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O46" s="3"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1">
@@ -2147,7 +2181,7 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
     </row>
-    <row r="47" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="47" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O47" s="3"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1">
@@ -2158,7 +2192,7 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
     </row>
-    <row r="48" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="48" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1">
@@ -2169,18 +2203,18 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="49" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="50" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1">
@@ -2191,7 +2225,7 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
     </row>
-    <row r="51" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="51" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1">
@@ -2202,7 +2236,7 @@
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
     </row>
-    <row r="52" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="52" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1">
@@ -2213,7 +2247,7 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
     </row>
-    <row r="53" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="53" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1">
@@ -2224,7 +2258,7 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
     </row>
-    <row r="54" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="54" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1">
@@ -2235,7 +2269,7 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
     </row>
-    <row r="55" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="55" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1">
@@ -2246,7 +2280,7 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
     </row>
-    <row r="56" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="56" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1">
@@ -2257,7 +2291,7 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
     </row>
-    <row r="57" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="57" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1">
@@ -2268,7 +2302,7 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
     </row>
-    <row r="58" spans="15:21" ht="15.75" hidden="1" customHeight="1">
+    <row r="58" spans="15:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1">
@@ -2279,7 +2313,7 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
     </row>
-    <row r="59" spans="15:21" ht="15.75" customHeight="1">
+    <row r="59" spans="15:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1">
@@ -2290,7 +2324,7 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
     </row>
-    <row r="60" spans="15:21" ht="15.75" customHeight="1">
+    <row r="60" spans="15:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1">
@@ -2301,11 +2335,11 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
     </row>
-    <row r="61" spans="15:21" ht="15.75" customHeight="1">
+    <row r="61" spans="15:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
@@ -2313,21 +2347,19 @@
       <c r="U61" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="23">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M9:N9"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="E12:G12"/>
@@ -2350,7 +2382,7 @@
     <dataValidation type="list" allowBlank="1" sqref="Z1" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$W:$W</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:L10 M10:O10" xr:uid="{F55BA1D6-8A5B-4E76-AF59-387396DE44F4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:O10" xr:uid="{F55BA1D6-8A5B-4E76-AF59-387396DE44F4}"/>
     <dataValidation type="list" allowBlank="1" sqref="E14" xr:uid="{F1164FB7-A39C-4E89-807C-721D7C318DB9}">
       <formula1>$N$32:$N$45</formula1>
     </dataValidation>

</xml_diff>